<commit_message>
ajout maquette et mcd
</commit_message>
<xml_diff>
--- a/TestsMaquettesFonctionnelles/Ambroise/Historique/maquette consulter l'historique des rapports de visite de sa région.xlsx
+++ b/TestsMaquettesFonctionnelles/Ambroise/Historique/maquette consulter l'historique des rapports de visite de sa région.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">1, 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Accès à l'historique des rapports régionaux. En allant sur la barre de navigation et dans historique à l’aide d’un compte Délégué 
+    <t xml:space="preserve">Accès à l'historique des rapports régionaux. En allant sur la barre de navigation, puis rapports et dans historique à l’aide d’un compte Délégué 
 Délégué ( login :leclud, mdp : LecLud!)</t>
   </si>
   <si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">3, 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Saisie des dates et validation (avec ou sans visiteur précisé).
+    <t xml:space="preserve">Saisie des dates et validation (avec ou sans visiteur précisé). Puis cliquer sur filtrer
 (choisir une période entre 2000 et 2026)
 </t>
   </si>
@@ -145,7 +145,7 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,42 +233,53 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2176560</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1732320</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:colOff>1731960</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="1" name="Image 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3066840" y="5742000"/>
-          <a:ext cx="9806400" cy="6688800"/>
+          <a:ext cx="9806040" cy="6688440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:blipFill rotWithShape="0">
           <a:blip r:embed="rId1"/>
+          <a:srcRect/>
           <a:stretch/>
         </a:blipFill>
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr" anchorCtr="1">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="fr-FR" sz="1200" strike="noStrike" u="none">
               <a:effectLst/>
@@ -291,42 +302,53 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2163960</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1724400</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>195840</xdr:rowOff>
+      <xdr:colOff>1724040</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Image 2"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3054240" y="12951000"/>
-          <a:ext cx="9811080" cy="4245120"/>
+          <a:ext cx="9810720" cy="4244760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:blipFill rotWithShape="0">
           <a:blip r:embed="rId2"/>
+          <a:srcRect/>
           <a:stretch/>
         </a:blipFill>
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr" anchorCtr="1">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="fr-FR" sz="1200" strike="noStrike" u="none">
               <a:effectLst/>
@@ -349,42 +371,53 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3486600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>221760</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:colOff>221400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Image 3"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14627520" y="7145280"/>
-          <a:ext cx="7716240" cy="5237640"/>
+          <a:ext cx="7715880" cy="5237280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:blipFill rotWithShape="0">
           <a:blip r:embed="rId3"/>
+          <a:srcRect/>
           <a:stretch/>
         </a:blipFill>
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr" anchorCtr="1">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="fr-FR" sz="1200" strike="noStrike" u="none">
               <a:effectLst/>
@@ -584,10 +617,10 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -621,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -643,61 +676,66 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="26.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>7</v>
+    <row r="8" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>